<commit_message>
feats: video_link, major name, hero responsive
</commit_message>
<xml_diff>
--- a/public/excel/Header Student.xlsx
+++ b/public/excel/Header Student.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive - Bina Nusantara\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gitbee-frontend\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDC2F05-9E8E-4C4D-8302-FA5EE22DC8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864645A4-CA95-436A-8D6C-7FBF806022C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{668F7D20-86A7-4407-92C3-C1CD8776CF92}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Campus</t>
-  </si>
-  <si>
-    <t>Binusian ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Student ID</t>
   </si>
@@ -50,25 +44,13 @@
     <t>Official Name</t>
   </si>
   <si>
-    <t>Program</t>
-  </si>
-  <si>
     <t>Term</t>
-  </si>
-  <si>
-    <t>Enrichment Track</t>
   </si>
   <si>
     <t>Course Code</t>
   </si>
   <si>
-    <t>Long Title</t>
-  </si>
-  <si>
     <t>Class Section</t>
-  </si>
-  <si>
-    <t>Email Mahasiswa</t>
   </si>
 </sst>
 </file>
@@ -451,19 +433,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020DB012-444B-4B55-9D5F-25BCEB6685F9}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -472,7 +454,7 @@
     <col min="11" max="11" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,24 +470,6 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>